<commit_message>
feat: add project crud basic operation
</commit_message>
<xml_diff>
--- a/src/uploads/templates/template_file.xlsx
+++ b/src/uploads/templates/template_file.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917CFD74-7987-4FE6-A292-C4B5B4656B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D92E3C-5AC2-42C9-89C6-A594627E017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="855" windowWidth="27105" windowHeight="14625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="5" r:id="rId1"/>
@@ -516,7 +516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -791,6 +791,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -907,9 +918,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -922,50 +930,53 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -990,84 +1001,7 @@
     <cellStyle name="Title" xfId="10" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Title 2" xfId="18" xr:uid="{3C225313-BB6D-4B9C-B9AC-2C8F3AE6419B}"/>
   </cellStyles>
-  <dxfs count="53">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="51">
     <dxf>
       <fill>
         <patternFill>
@@ -1190,6 +1124,69 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1500,43 +1497,43 @@
   </dxfs>
   <tableStyles count="6" defaultTableStyle="To-Do List" defaultPivotStyle="PivotStyleLight2">
     <tableStyle name="To Do List Pivot" table="0" count="11" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="52"/>
-      <tableStyleElement type="totalRow" dxfId="51"/>
-      <tableStyleElement type="firstRowStripe" dxfId="50"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="49"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="48"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="47"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="46"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="45"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="44"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="43"/>
-      <tableStyleElement type="pageFieldValues" dxfId="42"/>
+      <tableStyleElement type="headerRow" dxfId="50"/>
+      <tableStyleElement type="totalRow" dxfId="49"/>
+      <tableStyleElement type="firstRowStripe" dxfId="48"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="47"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="46"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="45"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="44"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="43"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="42"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="41"/>
+      <tableStyleElement type="pageFieldValues" dxfId="40"/>
     </tableStyle>
     <tableStyle name="To-Do List" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="41"/>
+      <tableStyleElement type="wholeTable" dxfId="39"/>
     </tableStyle>
     <tableStyle name="Business plan checklist with SWOT analysis" pivot="0" count="7" xr9:uid="{2D409609-E333-4337-973D-7901C6ACFDE2}">
-      <tableStyleElement type="wholeTable" dxfId="40"/>
-      <tableStyleElement type="headerRow" dxfId="39"/>
-      <tableStyleElement type="totalRow" dxfId="38"/>
-      <tableStyleElement type="firstColumn" dxfId="37"/>
-      <tableStyleElement type="lastColumn" dxfId="36"/>
-      <tableStyleElement type="firstRowStripe" dxfId="35"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="34"/>
+      <tableStyleElement type="wholeTable" dxfId="38"/>
+      <tableStyleElement type="headerRow" dxfId="37"/>
+      <tableStyleElement type="totalRow" dxfId="36"/>
+      <tableStyleElement type="firstColumn" dxfId="35"/>
+      <tableStyleElement type="lastColumn" dxfId="34"/>
+      <tableStyleElement type="firstRowStripe" dxfId="33"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="32"/>
     </tableStyle>
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{4FA14B01-0BED-4FCC-81F8-7E6FFCEBBAE2}">
-      <tableStyleElement type="headerRow" dxfId="33"/>
-      <tableStyleElement type="secondRowStripe" dxfId="32"/>
+      <tableStyleElement type="headerRow" dxfId="31"/>
+      <tableStyleElement type="secondRowStripe" dxfId="30"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="3" xr9:uid="{A879C2FF-807D-45C9-86A1-25F0B0262231}">
-      <tableStyleElement type="wholeTable" dxfId="31"/>
-      <tableStyleElement type="headerRow" dxfId="30"/>
-      <tableStyleElement type="secondRowStripe" dxfId="29"/>
+      <tableStyleElement type="wholeTable" dxfId="29"/>
+      <tableStyleElement type="headerRow" dxfId="28"/>
+      <tableStyleElement type="secondRowStripe" dxfId="27"/>
     </tableStyle>
     <tableStyle name="Table Style 3" pivot="0" count="3" xr9:uid="{F6A89878-6390-4C16-BB5E-54119F5DBBFD}">
-      <tableStyleElement type="wholeTable" dxfId="28"/>
-      <tableStyleElement type="headerRow" dxfId="27"/>
-      <tableStyleElement type="secondRowStripe" dxfId="26"/>
+      <tableStyleElement type="wholeTable" dxfId="26"/>
+      <tableStyleElement type="headerRow" dxfId="25"/>
+      <tableStyleElement type="secondRowStripe" dxfId="24"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1551,13 +1548,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{307EB1DD-9335-4732-9802-9E3960666E62}" name="ToDoList4" displayName="ToDoList4" ref="B3:F4" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{307EB1DD-9335-4732-9802-9E3960666E62}" name="ToDoList4" displayName="ToDoList4" ref="B3:F4" totalsRowShown="0" headerRowDxfId="14">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D1AA060A-0C34-4C54-ABA8-E2D07143D245}" name="Date changed" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{D1AA060A-0C34-4C54-ABA8-E2D07143D245}" name="Date changed" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{4C8C8C98-7B58-441D-9DD7-3D496F83B0EC}" name="Version Date"/>
-    <tableColumn id="3" xr3:uid="{7305E4AC-5226-4376-8417-07237B5752BD}" name="Version number" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{B8F9875C-29FE-48DD-8B8F-769BAF1E885F}" name="Action(A/M/D)" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{C45AC4B4-551B-4695-B0AD-4F24EA99F199}" name="Changed Statement" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{7305E4AC-5226-4376-8417-07237B5752BD}" name="Version number" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{B8F9875C-29FE-48DD-8B8F-769BAF1E885F}" name="Action(A/M/D)" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{C45AC4B4-551B-4695-B0AD-4F24EA99F199}" name="Changed Statement" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="To-Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1801,7 +1798,7 @@
   </sheetPr>
   <dimension ref="C2:J9"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="B4" zoomScale="145" zoomScaleNormal="160" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="145" zoomScaleNormal="160" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
@@ -1819,12 +1816,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -1834,31 +1831,31 @@
       <c r="C3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
     </row>
     <row r="4" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="1"/>
       <c r="H5" s="3"/>
       <c r="I5" s="4"/>
@@ -1867,11 +1864,11 @@
       <c r="C6" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="1"/>
       <c r="H6" s="3"/>
       <c r="I6" s="4"/>
@@ -1880,31 +1877,31 @@
       <c r="C7" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
     </row>
     <row r="8" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
     </row>
     <row r="9" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1918,7 +1915,7 @@
     <mergeCell ref="D3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="G5:J6">
-    <cfRule type="expression" dxfId="18" priority="11">
+    <cfRule type="expression" dxfId="23" priority="11">
       <formula>AND($H5=0,$H5&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1937,37 +1934,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="17" priority="9">
+    <cfRule type="expression" dxfId="22" priority="9">
       <formula>AND($H3=0,$H3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="16" priority="8">
+    <cfRule type="expression" dxfId="21" priority="8">
       <formula>AND($H4=0,$H4&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="15" priority="7">
+    <cfRule type="expression" dxfId="20" priority="7">
       <formula>AND($H5=0,$H5&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>AND($H6=0,$H6&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>AND($H7=0,$H7&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND($H8=0,$H8&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>AND($H9=0,$H9&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2062,13 +2059,13 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="72.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
@@ -2112,7 +2109,7 @@
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="10" priority="40">
+    <cfRule type="expression" dxfId="15" priority="40">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2142,8 +2139,8 @@
   </sheetPr>
   <dimension ref="B1:K52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A29" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2175,56 +2172,56 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:11" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="34" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="34"/>
+      <c r="E2" s="39"/>
       <c r="F2" s="13"/>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="43" t="s">
+      <c r="H2" s="38"/>
+      <c r="I2" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="44"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="34" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="G3" s="41" t="s">
+      <c r="E3" s="39"/>
+      <c r="G3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="34" t="s">
+      <c r="H3" s="38"/>
+      <c r="I3" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="34"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="34" t="s">
+      <c r="C4" s="38"/>
+      <c r="D4" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
+      <c r="E4" s="39"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
     </row>
     <row r="6" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B6" s="14" t="s">
@@ -2248,99 +2245,99 @@
       <c r="C8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
     </row>
     <row r="11" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
     </row>
     <row r="12" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
     </row>
     <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
@@ -2359,43 +2356,43 @@
       <c r="C16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.65">
       <c r="B19" s="15" t="s">
@@ -2412,27 +2409,27 @@
       <c r="K19" s="7"/>
     </row>
     <row r="20" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
       <c r="J20" s="22"/>
     </row>
     <row r="21" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
       <c r="J21" s="22"/>
     </row>
     <row r="22" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2444,38 +2441,38 @@
       <c r="B23" s="15"/>
     </row>
     <row r="24" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="35" t="s">
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35" t="s">
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34" t="s">
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34" t="s">
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
     </row>
     <row r="27" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B27" s="14" t="s">
@@ -2496,27 +2493,27 @@
       </c>
     </row>
     <row r="29" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
       <c r="J29" s="22"/>
     </row>
     <row r="30" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
       <c r="J30" s="22"/>
     </row>
     <row r="31" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2525,38 +2522,38 @@
       </c>
     </row>
     <row r="32" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="37"/>
-      <c r="D32" s="35" t="s">
+      <c r="C32" s="46"/>
+      <c r="D32" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35" t="s">
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
     </row>
     <row r="33" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="34" t="s">
+      <c r="B33" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34" t="s">
+      <c r="C33" s="39"/>
+      <c r="D33" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="45" t="s">
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="47"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="34"/>
     </row>
     <row r="34" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="s">
@@ -2564,38 +2561,38 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="35" t="s">
+      <c r="C35" s="46"/>
+      <c r="D35" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="38" t="s">
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="40"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="37"/>
     </row>
     <row r="36" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34" t="s">
+      <c r="C36" s="39"/>
+      <c r="D36" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="45" t="s">
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="47"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="23" t="s">
@@ -2606,38 +2603,38 @@
       <c r="J37" s="16"/>
     </row>
     <row r="38" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="35" t="s">
+      <c r="C38" s="46"/>
+      <c r="D38" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="38" t="s">
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="37"/>
     </row>
     <row r="39" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="34" t="s">
+      <c r="B39" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34" t="s">
+      <c r="C39" s="39"/>
+      <c r="D39" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="45" t="s">
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="47"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="23" t="s">
@@ -2648,38 +2645,38 @@
       <c r="J40" s="16"/>
     </row>
     <row r="41" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="37"/>
-      <c r="D41" s="35" t="s">
+      <c r="C41" s="46"/>
+      <c r="D41" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="38" t="s">
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="39"/>
-      <c r="I41" s="39"/>
-      <c r="J41" s="40"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="36"/>
+      <c r="J41" s="37"/>
     </row>
     <row r="42" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="34" t="s">
+      <c r="B42" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34" t="s">
+      <c r="C42" s="39"/>
+      <c r="D42" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="45" t="s">
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="H42" s="46"/>
-      <c r="I42" s="46"/>
-      <c r="J42" s="47"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="23"/>
@@ -2702,42 +2699,42 @@
     </row>
     <row r="45" spans="2:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="37"/>
+      <c r="C46" s="46"/>
       <c r="D46" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="38" t="s">
+      <c r="E46" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F46" s="39"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="38" t="s">
+      <c r="F46" s="36"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="40"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="34" t="s">
+      <c r="B47" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="34"/>
+      <c r="C47" s="39"/>
       <c r="D47" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="34" t="s">
+      <c r="E47" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="45" t="s">
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="I47" s="46"/>
-      <c r="J47" s="47"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="34"/>
     </row>
     <row r="49" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
       <c r="B49" s="14" t="s">
@@ -2754,45 +2751,95 @@
     </row>
     <row r="50" spans="2:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="37" t="s">
+      <c r="B51" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="37"/>
+      <c r="C51" s="46"/>
       <c r="D51" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="38" t="s">
+      <c r="E51" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F51" s="39"/>
-      <c r="G51" s="40"/>
-      <c r="H51" s="38" t="s">
+      <c r="F51" s="36"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="I51" s="39"/>
-      <c r="J51" s="40"/>
+      <c r="I51" s="36"/>
+      <c r="J51" s="37"/>
     </row>
     <row r="52" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="34" t="s">
+      <c r="B52" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="34"/>
+      <c r="C52" s="39"/>
       <c r="D52" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E52" s="34" t="s">
+      <c r="E52" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="45" t="s">
+      <c r="F52" s="39"/>
+      <c r="G52" s="39"/>
+      <c r="H52" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="I52" s="46"/>
-      <c r="J52" s="47"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="B20:I21"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B29:I30"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D13:J13"/>
     <mergeCell ref="H52:J52"/>
     <mergeCell ref="H51:J51"/>
     <mergeCell ref="H47:J47"/>
@@ -2809,56 +2856,6 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:K4"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B29:I30"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="G41:J41"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="B20:I21"/>
-    <mergeCell ref="D13:J13"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B4 G2:G4">
     <cfRule type="expression" dxfId="9" priority="57">
@@ -2926,6 +2923,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3225,36 +3251,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D35F6BBC-27EF-4E66-8888-56069E1BF9FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFE0BFEE-800D-4D37-8011-9A003F823113}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEE202D-7AB6-4312-B68E-6677B4ED3F6F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3273,24 +3290,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFE0BFEE-800D-4D37-8011-9A003F823113}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D35F6BBC-27EF-4E66-8888-56069E1BF9FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: adding excel template export & fix project missing 2 attributes
</commit_message>
<xml_diff>
--- a/src/uploads/templates/template_file.xlsx
+++ b/src/uploads/templates/template_file.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D92E3C-5AC2-42C9-89C6-A594627E017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD05932-12BB-4B59-9658-050CA7D55A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="855" windowWidth="27105" windowHeight="14625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="5" r:id="rId1"/>
@@ -204,9 +204,6 @@
     <t>{project.division.code}</t>
   </si>
   <si>
-    <t>{project.createdBy.username}</t>
-  </si>
-  <si>
     <t>{templateData.versionDate}</t>
   </si>
   <si>
@@ -322,6 +319,9 @@
   </si>
   <si>
     <t>{project.opportunity.presale.version}</t>
+  </si>
+  <si>
+    <t>{project.lead.username}</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -564,15 +564,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="hair">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="hair">
         <color indexed="64"/>
       </left>
@@ -802,6 +793,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -832,18 +871,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -860,11 +899,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="10" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1"/>
@@ -874,10 +910,10 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="10" applyFont="1"/>
@@ -888,16 +924,16 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="2" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="2" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="2" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyBorder="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -909,26 +945,56 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="10" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="10" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -936,47 +1002,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1001,76 +1052,28 @@
     <cellStyle name="Title" xfId="10" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Title 2" xfId="18" xr:uid="{3C225313-BB6D-4B9C-B9AC-2C8F3AE6419B}"/>
   </cellStyles>
-  <dxfs count="51">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
+  <dxfs count="52">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="hair">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="hair">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1087,6 +1090,90 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="hair">
           <color indexed="64"/>
@@ -1104,18 +1191,6 @@
           <color indexed="64"/>
         </left>
         <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
         <top/>
         <bottom/>
         <vertical/>
@@ -1497,43 +1572,43 @@
   </dxfs>
   <tableStyles count="6" defaultTableStyle="To-Do List" defaultPivotStyle="PivotStyleLight2">
     <tableStyle name="To Do List Pivot" table="0" count="11" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="50"/>
-      <tableStyleElement type="totalRow" dxfId="49"/>
-      <tableStyleElement type="firstRowStripe" dxfId="48"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="47"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="46"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="45"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="44"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="43"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="42"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="41"/>
-      <tableStyleElement type="pageFieldValues" dxfId="40"/>
+      <tableStyleElement type="headerRow" dxfId="51"/>
+      <tableStyleElement type="totalRow" dxfId="50"/>
+      <tableStyleElement type="firstRowStripe" dxfId="49"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="48"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="47"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="46"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="45"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="44"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="43"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="42"/>
+      <tableStyleElement type="pageFieldValues" dxfId="41"/>
     </tableStyle>
     <tableStyle name="To-Do List" pivot="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="wholeTable" dxfId="39"/>
+      <tableStyleElement type="wholeTable" dxfId="40"/>
     </tableStyle>
     <tableStyle name="Business plan checklist with SWOT analysis" pivot="0" count="7" xr9:uid="{2D409609-E333-4337-973D-7901C6ACFDE2}">
-      <tableStyleElement type="wholeTable" dxfId="38"/>
-      <tableStyleElement type="headerRow" dxfId="37"/>
-      <tableStyleElement type="totalRow" dxfId="36"/>
-      <tableStyleElement type="firstColumn" dxfId="35"/>
-      <tableStyleElement type="lastColumn" dxfId="34"/>
-      <tableStyleElement type="firstRowStripe" dxfId="33"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="32"/>
+      <tableStyleElement type="wholeTable" dxfId="39"/>
+      <tableStyleElement type="headerRow" dxfId="38"/>
+      <tableStyleElement type="totalRow" dxfId="37"/>
+      <tableStyleElement type="firstColumn" dxfId="36"/>
+      <tableStyleElement type="lastColumn" dxfId="35"/>
+      <tableStyleElement type="firstRowStripe" dxfId="34"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="33"/>
     </tableStyle>
     <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{4FA14B01-0BED-4FCC-81F8-7E6FFCEBBAE2}">
-      <tableStyleElement type="headerRow" dxfId="31"/>
-      <tableStyleElement type="secondRowStripe" dxfId="30"/>
+      <tableStyleElement type="headerRow" dxfId="32"/>
+      <tableStyleElement type="secondRowStripe" dxfId="31"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="3" xr9:uid="{A879C2FF-807D-45C9-86A1-25F0B0262231}">
-      <tableStyleElement type="wholeTable" dxfId="29"/>
-      <tableStyleElement type="headerRow" dxfId="28"/>
-      <tableStyleElement type="secondRowStripe" dxfId="27"/>
+      <tableStyleElement type="wholeTable" dxfId="30"/>
+      <tableStyleElement type="headerRow" dxfId="29"/>
+      <tableStyleElement type="secondRowStripe" dxfId="28"/>
     </tableStyle>
     <tableStyle name="Table Style 3" pivot="0" count="3" xr9:uid="{F6A89878-6390-4C16-BB5E-54119F5DBBFD}">
-      <tableStyleElement type="wholeTable" dxfId="26"/>
-      <tableStyleElement type="headerRow" dxfId="25"/>
-      <tableStyleElement type="secondRowStripe" dxfId="24"/>
+      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="secondRowStripe" dxfId="25"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1548,13 +1623,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{307EB1DD-9335-4732-9802-9E3960666E62}" name="ToDoList4" displayName="ToDoList4" ref="B3:F4" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{307EB1DD-9335-4732-9802-9E3960666E62}" name="ToDoList4" displayName="ToDoList4" ref="B3:F4" totalsRowShown="0" headerRowDxfId="15">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{D1AA060A-0C34-4C54-ABA8-E2D07143D245}" name="Date changed" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{4C8C8C98-7B58-441D-9DD7-3D496F83B0EC}" name="Version Date"/>
-    <tableColumn id="3" xr3:uid="{7305E4AC-5226-4376-8417-07237B5752BD}" name="Version number" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{B8F9875C-29FE-48DD-8B8F-769BAF1E885F}" name="Action(A/M/D)" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{C45AC4B4-551B-4695-B0AD-4F24EA99F199}" name="Changed Statement" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{D1AA060A-0C34-4C54-ABA8-E2D07143D245}" name="Date changed" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{4C8C8C98-7B58-441D-9DD7-3D496F83B0EC}" name="Version Date" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{7305E4AC-5226-4376-8417-07237B5752BD}" name="Version number" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{B8F9875C-29FE-48DD-8B8F-769BAF1E885F}" name="Action(A/M/D)" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{C45AC4B4-551B-4695-B0AD-4F24EA99F199}" name="Changed Statement" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="To-Do List" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
   <extLst>
@@ -1798,7 +1873,7 @@
   </sheetPr>
   <dimension ref="C2:J9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="145" zoomScaleNormal="160" zoomScaleSheetLayoutView="145" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="145" zoomScaleNormal="160" zoomScaleSheetLayoutView="145" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:F4"/>
     </sheetView>
   </sheetViews>
@@ -1816,8 +1891,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="C2" s="47" t="s">
-        <v>61</v>
+      <c r="C2" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
@@ -1828,27 +1903,27 @@
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="49"/>
     </row>
     <row r="4" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="25" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
     </row>
     <row r="5" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="30" t="s">
@@ -1861,7 +1936,7 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="30" t="s">
@@ -1874,7 +1949,7 @@
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="30" t="s">
@@ -1884,7 +1959,7 @@
       <c r="F7" s="30"/>
     </row>
     <row r="8" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="25" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="30" t="s">
@@ -1894,11 +1969,11 @@
       <c r="F8" s="30"/>
     </row>
     <row r="9" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
@@ -1915,7 +1990,7 @@
     <mergeCell ref="D3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="G5:J6">
-    <cfRule type="expression" dxfId="23" priority="11">
+    <cfRule type="expression" dxfId="24" priority="11">
       <formula>AND($H5=0,$H5&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1934,37 +2009,37 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="22" priority="9">
+    <cfRule type="expression" dxfId="23" priority="9">
       <formula>AND($H3=0,$H3&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="21" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>AND($H4=0,$H4&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="20" priority="7">
+    <cfRule type="expression" dxfId="21" priority="7">
       <formula>AND($H5=0,$H5&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="19" priority="5">
+    <cfRule type="expression" dxfId="20" priority="5">
       <formula>AND($H6=0,$H6&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="19" priority="4">
       <formula>AND($H7=0,$H7&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>AND($H8=0,$H8&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>AND($H9=0,$H9&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2030,10 +2105,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="D1" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="205" zoomScaleNormal="100" zoomScaleSheetLayoutView="205" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2131,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="11"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" ht="72.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="31" t="s">
@@ -2066,50 +2141,53 @@
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
-      <c r="G2" s="10"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>60</v>
-      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:F2"/>
   </mergeCells>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="15" priority="40">
+    <cfRule type="expression" dxfId="16" priority="40">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2172,59 +2250,59 @@
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="2:11" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="45"/>
+      <c r="I2" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="44"/>
+    </row>
+    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="45"/>
+      <c r="D3" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="36"/>
+      <c r="G3" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="45"/>
+      <c r="I3" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="36"/>
+    </row>
+    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="45"/>
+      <c r="D4" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="39"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="38"/>
-      <c r="I2" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="43"/>
-    </row>
-    <row r="3" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="39"/>
-      <c r="G3" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="39"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="41"/>
-      <c r="K4" s="41"/>
+      <c r="E4" s="36"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
     </row>
     <row r="6" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2"/>
@@ -2237,245 +2315,245 @@
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="2:11" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+    </row>
+    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+    </row>
+    <row r="12" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-    </row>
-    <row r="9" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
-    </row>
-    <row r="10" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="17" t="s">
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+    </row>
+    <row r="14" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+    </row>
+    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+    </row>
+    <row r="17" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-    </row>
-    <row r="11" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-    </row>
-    <row r="12" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-    </row>
-    <row r="13" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="40" t="s">
-        <v>90</v>
-      </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-    </row>
-    <row r="14" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-    </row>
-    <row r="15" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="17" t="s">
+      <c r="D17" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.65">
+      <c r="B19" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="21"/>
+    </row>
+    <row r="21" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="14"/>
+    </row>
+    <row r="24" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-    </row>
-    <row r="17" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-    </row>
-    <row r="18" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-    </row>
-    <row r="19" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="B19" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="44"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="22"/>
-    </row>
-    <row r="21" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="22"/>
-    </row>
-    <row r="22" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-    </row>
-    <row r="24" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="45" t="s">
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45" t="s">
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39" t="s">
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
     </row>
     <row r="27" spans="2:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="2"/>
@@ -2488,204 +2566,204 @@
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="2:11" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="22"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="21"/>
     </row>
     <row r="30" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="22"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="21"/>
     </row>
     <row r="31" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="23" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="32" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="46"/>
-      <c r="D32" s="45" t="s">
+      <c r="C32" s="32"/>
+      <c r="D32" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45" t="s">
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
     </row>
     <row r="33" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="39" t="s">
+      <c r="B33" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39" t="s">
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="42"/>
+    </row>
+    <row r="34" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="32"/>
+      <c r="D35" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="35"/>
+    </row>
+    <row r="36" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="34"/>
-    </row>
-    <row r="34" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="46" t="s">
+      <c r="C36" s="36"/>
+      <c r="D36" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="42"/>
+    </row>
+    <row r="37" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+    </row>
+    <row r="38" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="46"/>
-      <c r="D35" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="37"/>
-    </row>
-    <row r="36" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="39"/>
-      <c r="D36" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
-      <c r="G36" s="32" t="s">
+      <c r="C38" s="32"/>
+      <c r="D38" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="35"/>
+    </row>
+    <row r="39" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="34"/>
-    </row>
-    <row r="37" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-    </row>
-    <row r="38" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="46" t="s">
+      <c r="C39" s="36"/>
+      <c r="D39" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="42"/>
+    </row>
+    <row r="40" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+    </row>
+    <row r="41" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
-    </row>
-    <row r="39" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="39"/>
-      <c r="D39" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="32" t="s">
+      <c r="C41" s="32"/>
+      <c r="D41" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="35"/>
+    </row>
+    <row r="42" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="33"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="34"/>
-    </row>
-    <row r="40" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-    </row>
-    <row r="41" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
-    </row>
-    <row r="42" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39" t="s">
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="34"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="42"/>
     </row>
     <row r="43" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="23"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
+      <c r="B43" s="22"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
     </row>
     <row r="44" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="2"/>
@@ -2699,45 +2777,45 @@
     </row>
     <row r="45" spans="2:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="46" t="s">
+      <c r="B46" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="46"/>
-      <c r="D46" s="25" t="s">
+      <c r="C46" s="32"/>
+      <c r="D46" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E46" s="35" t="s">
+      <c r="E46" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="F46" s="36"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="35" t="s">
+      <c r="F46" s="34"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="37"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="35"/>
     </row>
     <row r="47" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="39" t="s">
+      <c r="B47" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C47" s="36"/>
+      <c r="D47" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C47" s="39"/>
-      <c r="D47" s="18" t="s">
+      <c r="E47" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="E47" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="I47" s="33"/>
-      <c r="J47" s="34"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="I47" s="41"/>
+      <c r="J47" s="42"/>
     </row>
     <row r="49" spans="2:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.7">
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="13" t="s">
         <v>43</v>
       </c>
       <c r="C49" s="2"/>
@@ -2751,45 +2829,95 @@
     </row>
     <row r="50" spans="2:10" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="46"/>
-      <c r="D51" s="25" t="s">
+      <c r="C51" s="32"/>
+      <c r="D51" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E51" s="35" t="s">
+      <c r="E51" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F51" s="36"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="35" t="s">
+      <c r="F51" s="34"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="I51" s="36"/>
-      <c r="J51" s="37"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="35"/>
     </row>
     <row r="52" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="39" t="s">
+      <c r="B52" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="36"/>
+      <c r="D52" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="39"/>
-      <c r="D52" s="18" t="s">
+      <c r="E52" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="E52" s="39" t="s">
+      <c r="F52" s="36"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="F52" s="39"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="I52" s="33"/>
-      <c r="J52" s="34"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B29:I30"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D10:J10"/>
+    <mergeCell ref="D14:J14"/>
+    <mergeCell ref="D12:J12"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="D38:F38"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="E51:G51"/>
     <mergeCell ref="B52:C52"/>
@@ -2806,104 +2934,54 @@
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="D33:F33"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="G41:J41"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="B29:I30"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D17:J17"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B4 G2:G4">
-    <cfRule type="expression" dxfId="9" priority="57">
+    <cfRule type="expression" dxfId="11" priority="57">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="8" priority="14">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="2" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>AND(#REF!=0,#REF!&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2923,35 +3001,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="26" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ac37c1753acd5e330d2062ccec26ea66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b340c7101c92c5120abd06486f94548" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3251,27 +3300,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D35F6BBC-27EF-4E66-8888-56069E1BF9FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFE0BFEE-800D-4D37-8011-9A003F823113}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DEE202D-7AB6-4312-B68E-6677B4ED3F6F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3290,4 +3348,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFE0BFEE-800D-4D37-8011-9A003F823113}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D35F6BBC-27EF-4E66-8888-56069E1BF9FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>